<commit_message>
update dqc_0011 list of elements
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
+++ b/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
@@ -481,7 +481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
@@ -551,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="6">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
@@ -571,7 +573,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">

</xml_diff>

<commit_message>
Update v11 for rules team post-implementation fixes (#458)
* Updated for extensible list values for current or noncurrent

* Updated rule 87 for bug fixes

* Updated V11 for changes in rule 87

* Update DQC_0087.xule

* Update dqc-us-2019-V11-ruleset.zip

* Push Changes to 83 for xule errors.

* Updated Rulesets for 8-k exclusion on rule 83

* update .travis.yml for dqc_0087 tests

* Update dqc_0085 unit test

* update dqc_0011 list of elements

* Update rulesetMap.json to correct paths for 2011-15 UGT references

Co-authored-by: Campbell Pryde <campbell.pryde@xbrl.us>
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
+++ b/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
@@ -481,7 +481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
@@ -551,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="6">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
@@ -571,7 +573,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">

</xml_diff>

<commit_message>
Update v12 for public exposure (#468)
* Updated V12 ruleset

* update dqc_0011 list of elements

* Update to Rule 48

* Updated rule 45 and updated effective date list for US and IFRS

* Updated V11 for effective dates

* Updates for version 12 for effective date issues.

* Recompiled code for effective date changes.

* 2020 Taxonomy added to version 11.

* Create dqc-us-2020-V11-ruleset.zip

* Updated 2020 for changes

* Updated V12 Rules for Xule errors

* Updated V12 rules

* Updated DQC 0001.70 for new allowable extension items

* Updated rules for version 12

* Updated V12 rules based on rule logic forms

* Update docs from v11

* Add v12 rule submission forms

* Update fix relative links

* Update fix line breaks

Co-authored-by: campbellpryde <campbell.pryde@xbrl.us>
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
+++ b/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
@@ -481,7 +481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
@@ -551,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="6">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
@@ -571,7 +573,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">

</xml_diff>

<commit_message>
Update for v19 Approved
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
+++ b/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BFF431-D7B6-CD46-AADC-B42D9E6BC808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="520" windowWidth="35320" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="525" windowWidth="28455" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="New Section" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>LineItem</t>
   </si>
@@ -127,8 +121,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -178,17 +172,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -197,14 +191,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -251,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,27 +269,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,24 +303,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -528,25 +478,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.3984375" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" style="3"/>
-    <col min="2" max="2" width="98.3984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="126" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31.3984375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="49.3984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.3984375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="21.3984375" style="3"/>
+    <col min="1" max="1" width="21.5" style="3"/>
+    <col min="2" max="2" width="98.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="66.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="21.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="15.95" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -566,7 +516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
       <c r="A2" s="7">
         <v>6820</v>
       </c>
@@ -586,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
       <c r="A3" s="7">
         <v>6821</v>
       </c>
@@ -606,7 +556,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
       <c r="A4" s="7">
         <v>6822</v>
       </c>
@@ -626,169 +576,169 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
       <c r="A5" s="7">
+        <v>6823</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A6" s="7">
         <v>6824</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A7" s="7">
         <v>6825</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A8" s="7">
         <v>6826</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7">
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A9" s="7">
         <v>6827</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F9" s="6">
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
+    <row r="10" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A10" s="7">
         <v>6828</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A11" s="7">
         <v>6829</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A12" s="7">
         <v>6830</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A13" s="7">
         <v>6831</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="7">
-        <v>6832</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
@@ -800,67 +750,47 @@
         <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A14" s="7">
+        <v>6832</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5">
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A15" s="5">
         <v>9292</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F14" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="5">
-        <v>9293</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F15" s="6">
         <v>-1</v>
@@ -886,6 +816,46 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+      <c r="A16" s="5">
+        <v>9293</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="6">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update from DQC v19.0.1
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
+++ b/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BFF431-D7B6-CD46-AADC-B42D9E6BC808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="525" windowWidth="28455" windowHeight="12210"/>
+    <workbookView xWindow="160" yWindow="520" windowWidth="35320" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Section" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>LineItem</t>
   </si>
@@ -121,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -172,17 +178,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -191,6 +197,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -237,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,9 +283,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,6 +335,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,25 +528,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="15.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.3984375" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="3"/>
-    <col min="2" max="2" width="98.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="49.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="21.5" style="3"/>
+    <col min="1" max="1" width="21.3984375" style="3"/>
+    <col min="2" max="2" width="98.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="126" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.3984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49.3984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.3984375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="21.3984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.95" customHeight="1">
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -516,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="2" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7">
         <v>6820</v>
       </c>
@@ -536,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="3" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7">
         <v>6821</v>
       </c>
@@ -556,7 +606,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="4" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>6822</v>
       </c>
@@ -576,12 +626,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="5" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
-        <v>6823</v>
+        <v>6824</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
@@ -590,18 +640,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="6" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
-        <v>6824</v>
+        <v>6825</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
@@ -610,18 +660,18 @@
         <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="7" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
-        <v>6825</v>
+        <v>6826</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>6</v>
@@ -630,18 +680,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
-        <v>6826</v>
+        <v>6827</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>6</v>
@@ -650,18 +700,18 @@
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
-        <v>6827</v>
+        <v>6828</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
@@ -670,18 +720,18 @@
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F9" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
-        <v>6828</v>
+        <v>6829</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
@@ -690,55 +740,55 @@
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>6830</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>6831</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A11" s="7">
-        <v>6829</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A12" s="7">
-        <v>6830</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="F12" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
-        <v>6831</v>
+        <v>6832</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
@@ -750,38 +800,58 @@
         <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F13" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A14" s="7">
-        <v>6832</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>24</v>
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>9292</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
-        <v>9292</v>
+        <v>9293</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -790,7 +860,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F15" s="6">
         <v>-1</v>
@@ -816,46 +886,6 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A16" s="5">
-        <v>9293</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Added documentation to Repo
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
+++ b/docs/DQC_US_0011/DQC_011_ListOfElements.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BFF431-D7B6-CD46-AADC-B42D9E6BC808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="525" windowWidth="28455" windowHeight="12210"/>
+    <workbookView xWindow="160" yWindow="520" windowWidth="35320" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Section" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>LineItem</t>
   </si>
@@ -121,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -172,17 +178,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -191,6 +197,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -237,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,9 +283,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,6 +335,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,25 +528,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.5" defaultRowHeight="15.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.3984375" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="3"/>
-    <col min="2" max="2" width="98.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="49.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="21.5" style="3"/>
+    <col min="1" max="1" width="21.3984375" style="3"/>
+    <col min="2" max="2" width="98.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="126" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.3984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49.3984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.3984375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="21.3984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.95" customHeight="1">
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -516,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="2" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7">
         <v>6820</v>
       </c>
@@ -536,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="3" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7">
         <v>6821</v>
       </c>
@@ -556,7 +606,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="4" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
         <v>6822</v>
       </c>
@@ -576,12 +626,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="5" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
-        <v>6823</v>
+        <v>6824</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
@@ -590,18 +640,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="6" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
-        <v>6824</v>
+        <v>6825</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
@@ -610,18 +660,18 @@
         <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="7" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
-        <v>6825</v>
+        <v>6826</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>6</v>
@@ -630,18 +680,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
-        <v>6826</v>
+        <v>6827</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>6</v>
@@ -650,18 +700,18 @@
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
-        <v>6827</v>
+        <v>6828</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
@@ -670,18 +720,18 @@
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F9" s="6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
-        <v>6828</v>
+        <v>6829</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
@@ -690,55 +740,55 @@
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>6830</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>6831</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A11" s="7">
-        <v>6829</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A12" s="7">
-        <v>6830</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="F12" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
-        <v>6831</v>
+        <v>6832</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
@@ -750,38 +800,58 @@
         <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F13" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A14" s="7">
-        <v>6832</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>24</v>
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>9292</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
-        <v>9292</v>
+        <v>9293</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -790,7 +860,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F15" s="6">
         <v>-1</v>
@@ -816,46 +886,6 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" s="4" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A16" s="5">
-        <v>9293</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="6">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>